<commit_message>
エラー詳細コード追加しました。 InvoiceDuplication OrderNotExist InvoiceNotExist
</commit_message>
<xml_diff>
--- a/invoice-doc/10_基本設計/API仕様書.xlsx
+++ b/invoice-doc/10_基本設計/API仕様書.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\invoice\invoice-doc\10_基本設計\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="請求書一覧取得" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="235">
   <si>
     <t>リクエストヘッダー</t>
     <phoneticPr fontId="1"/>
@@ -1303,12 +1308,40 @@
     <t>文字種チェックエラー</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>InvoiceDuplication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>請求書の期間が重複しています。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>存在チェックエラー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OrderNotExist</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>注文実績が存在しません。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>請求書が存在しません。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InvoiceNotExist</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1356,7 +1389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1379,6 +1412,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1388,7 +1458,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1452,14 +1522,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3837,13 +3919,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>191396</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4220,7 +4302,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4232,23 +4314,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -4256,7 +4338,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4264,32 +4346,32 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
@@ -4302,16 +4384,16 @@
       <c r="E15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="2:11">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
@@ -4322,16 +4404,16 @@
         <v>33</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="2:11">
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
         <v>74</v>
       </c>
@@ -4342,16 +4424,16 @@
         <v>33</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>150</v>
       </c>
@@ -4362,14 +4444,14 @@
         <v>33</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>217</v>
       </c>
@@ -4380,16 +4462,16 @@
         <v>33</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" spans="2:11" ht="27" customHeight="1">
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
         <v>140</v>
       </c>
@@ -4400,16 +4482,16 @@
         <v>33</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="2:11" ht="27" customHeight="1">
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+    </row>
+    <row r="21" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>141</v>
       </c>
@@ -4420,21 +4502,21 @@
         <v>33</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
@@ -4442,7 +4524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
@@ -4450,12 +4532,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
@@ -4465,17 +4547,17 @@
       <c r="D28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-    </row>
-    <row r="29" spans="2:11">
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B29" s="1" t="s">
         <v>161</v>
       </c>
@@ -4485,15 +4567,15 @@
       <c r="D29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-    </row>
-    <row r="30" spans="2:11">
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30" s="1" t="s">
         <v>158</v>
       </c>
@@ -4503,17 +4585,17 @@
       <c r="D30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" s="1" t="s">
         <v>154</v>
       </c>
@@ -4523,15 +4605,15 @@
       <c r="D31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-    </row>
-    <row r="32" spans="2:11">
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" s="1" t="s">
         <v>87</v>
       </c>
@@ -4541,15 +4623,15 @@
       <c r="D32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-    </row>
-    <row r="33" spans="2:11">
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B33" s="1" t="s">
         <v>151</v>
       </c>
@@ -4559,15 +4641,15 @@
       <c r="D33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-    </row>
-    <row r="34" spans="2:11">
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
         <v>152</v>
       </c>
@@ -4577,15 +4659,15 @@
       <c r="D34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-    </row>
-    <row r="35" spans="2:11">
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
         <v>89</v>
       </c>
@@ -4595,15 +4677,15 @@
       <c r="D35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="2:11">
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
@@ -4613,15 +4695,15 @@
       <c r="D36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
         <v>133</v>
       </c>
@@ -4631,17 +4713,17 @@
       <c r="D37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-    </row>
-    <row r="38" spans="2:11">
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B38" s="1" t="s">
         <v>91</v>
       </c>
@@ -4651,17 +4733,17 @@
       <c r="D38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39" spans="2:11">
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B39" s="1" t="s">
         <v>92</v>
       </c>
@@ -4671,17 +4753,17 @@
       <c r="D39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-    </row>
-    <row r="40" spans="2:11">
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B40" s="1" t="s">
         <v>93</v>
       </c>
@@ -4691,15 +4773,15 @@
       <c r="D40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="41" spans="2:11">
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B41" s="1" t="s">
         <v>94</v>
       </c>
@@ -4709,15 +4791,15 @@
       <c r="D41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-    </row>
-    <row r="42" spans="2:11">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B42" s="1" t="s">
         <v>95</v>
       </c>
@@ -4727,17 +4809,17 @@
       <c r="D42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-    </row>
-    <row r="43" spans="2:11">
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B43" s="1" t="s">
         <v>96</v>
       </c>
@@ -4747,17 +4829,17 @@
       <c r="D43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-    </row>
-    <row r="44" spans="2:11">
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B44" s="1" t="s">
         <v>97</v>
       </c>
@@ -4767,17 +4849,17 @@
       <c r="D44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-    </row>
-    <row r="45" spans="2:11">
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B45" s="1" t="s">
         <v>98</v>
       </c>
@@ -4787,15 +4869,15 @@
       <c r="D45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-    </row>
-    <row r="46" spans="2:11">
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B46" s="1" t="s">
         <v>99</v>
       </c>
@@ -4805,15 +4887,15 @@
       <c r="D46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-    </row>
-    <row r="47" spans="2:11">
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
@@ -4823,17 +4905,17 @@
       <c r="D47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-    </row>
-    <row r="48" spans="2:11">
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B48" s="1" t="s">
         <v>101</v>
       </c>
@@ -4843,15 +4925,15 @@
       <c r="D48" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-    </row>
-    <row r="49" spans="2:11">
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B49" s="1" t="s">
         <v>102</v>
       </c>
@@ -4861,17 +4943,17 @@
       <c r="D49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
-    </row>
-    <row r="50" spans="2:11">
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B50" s="1" t="s">
         <v>103</v>
       </c>
@@ -4881,32 +4963,33 @@
       <c r="D50" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-    </row>
-    <row r="52" spans="2:11">
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="E31:K31"/>
-    <mergeCell ref="E30:K30"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="E47:K47"/>
+    <mergeCell ref="E48:K48"/>
+    <mergeCell ref="E49:K49"/>
+    <mergeCell ref="E50:K50"/>
+    <mergeCell ref="E41:K41"/>
+    <mergeCell ref="E42:K42"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="E44:K44"/>
+    <mergeCell ref="E45:K45"/>
+    <mergeCell ref="E46:K46"/>
     <mergeCell ref="E40:K40"/>
     <mergeCell ref="E28:K28"/>
     <mergeCell ref="E29:K29"/>
@@ -4918,16 +5001,15 @@
     <mergeCell ref="E36:K36"/>
     <mergeCell ref="E38:K38"/>
     <mergeCell ref="E39:K39"/>
-    <mergeCell ref="E47:K47"/>
-    <mergeCell ref="E48:K48"/>
-    <mergeCell ref="E49:K49"/>
-    <mergeCell ref="E50:K50"/>
-    <mergeCell ref="E41:K41"/>
-    <mergeCell ref="E42:K42"/>
-    <mergeCell ref="E43:K43"/>
-    <mergeCell ref="E44:K44"/>
-    <mergeCell ref="E45:K45"/>
-    <mergeCell ref="E46:K46"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="E31:K31"/>
+    <mergeCell ref="E30:K30"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -4946,23 +5028,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -4970,7 +5052,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
@@ -4978,32 +5060,32 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
@@ -5011,7 +5093,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -5019,12 +5101,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
@@ -5034,16 +5116,16 @@
       <c r="D19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
@@ -5053,14 +5135,14 @@
       <c r="D20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>150</v>
       </c>
@@ -5070,14 +5152,14 @@
       <c r="D21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
         <v>53</v>
       </c>
@@ -5087,14 +5169,14 @@
       <c r="D22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>54</v>
       </c>
@@ -5104,14 +5186,14 @@
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="2:11">
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
@@ -5121,14 +5203,14 @@
       <c r="D24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="2:11">
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
@@ -5138,14 +5220,14 @@
       <c r="D25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="2:11">
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
@@ -5155,14 +5237,14 @@
       <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
         <v>131</v>
       </c>
@@ -5172,17 +5254,17 @@
       <c r="D27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
@@ -5192,16 +5274,16 @@
       <c r="D28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="2:11">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
@@ -5211,16 +5293,16 @@
       <c r="D29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="2:11">
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30" s="1" t="s">
         <v>57</v>
       </c>
@@ -5230,14 +5312,14 @@
       <c r="D30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
@@ -5247,14 +5329,14 @@
       <c r="D31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="2:11">
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" s="1" t="s">
         <v>120</v>
       </c>
@@ -5264,16 +5346,16 @@
       <c r="D32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="2:10">
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B33" s="1" t="s">
         <v>59</v>
       </c>
@@ -5283,16 +5365,16 @@
       <c r="D33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="34" spans="2:10">
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
@@ -5302,16 +5384,16 @@
       <c r="D34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="2:10">
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
         <v>61</v>
       </c>
@@ -5321,14 +5403,14 @@
       <c r="D35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="2:10">
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
         <v>62</v>
       </c>
@@ -5338,14 +5420,14 @@
       <c r="D36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-    </row>
-    <row r="37" spans="2:10">
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
         <v>63</v>
       </c>
@@ -5355,16 +5437,16 @@
       <c r="D37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-    </row>
-    <row r="38" spans="2:10">
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" s="1" t="s">
         <v>64</v>
       </c>
@@ -5374,14 +5456,14 @@
       <c r="D38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-    </row>
-    <row r="39" spans="2:10">
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" s="1" t="s">
         <v>65</v>
       </c>
@@ -5391,16 +5473,16 @@
       <c r="D39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-    </row>
-    <row r="40" spans="2:10">
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" s="6" t="s">
         <v>155</v>
       </c>
@@ -5410,14 +5492,14 @@
       <c r="D40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-    </row>
-    <row r="41" spans="2:10">
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" s="6" t="s">
         <v>105</v>
       </c>
@@ -5427,14 +5509,14 @@
       <c r="D41" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-    </row>
-    <row r="42" spans="2:10">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" s="6" t="s">
         <v>106</v>
       </c>
@@ -5444,14 +5526,14 @@
       <c r="D42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-    </row>
-    <row r="43" spans="2:10">
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" s="6" t="s">
         <v>107</v>
       </c>
@@ -5461,14 +5543,14 @@
       <c r="D43" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-    </row>
-    <row r="44" spans="2:10">
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B44" s="6" t="s">
         <v>134</v>
       </c>
@@ -5478,16 +5560,16 @@
       <c r="D44" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-    </row>
-    <row r="45" spans="2:10">
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B45" s="6" t="s">
         <v>108</v>
       </c>
@@ -5497,16 +5579,16 @@
       <c r="D45" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-    </row>
-    <row r="46" spans="2:10">
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B46" s="6" t="s">
         <v>109</v>
       </c>
@@ -5516,14 +5598,14 @@
       <c r="D46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-    </row>
-    <row r="47" spans="2:10">
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
         <v>110</v>
       </c>
@@ -5533,14 +5615,14 @@
       <c r="D47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="48" spans="2:10">
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B48" s="6" t="s">
         <v>111</v>
       </c>
@@ -5550,16 +5632,16 @@
       <c r="D48" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-    </row>
-    <row r="49" spans="2:10">
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B49" s="6" t="s">
         <v>112</v>
       </c>
@@ -5569,22 +5651,37 @@
       <c r="D49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-    </row>
-    <row r="51" spans="2:10" ht="27">
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B51" s="8" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="E46:J46"/>
+    <mergeCell ref="E47:J47"/>
+    <mergeCell ref="E48:J48"/>
+    <mergeCell ref="E49:J49"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
     <mergeCell ref="E19:J19"/>
     <mergeCell ref="E44:J44"/>
     <mergeCell ref="E40:J40"/>
@@ -5601,21 +5698,6 @@
     <mergeCell ref="E25:J25"/>
     <mergeCell ref="E26:J26"/>
     <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E43:J43"/>
-    <mergeCell ref="E45:J45"/>
-    <mergeCell ref="E46:J46"/>
-    <mergeCell ref="E47:J47"/>
-    <mergeCell ref="E48:J48"/>
-    <mergeCell ref="E49:J49"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -5633,24 +5715,24 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5658,7 +5740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
@@ -5666,12 +5748,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
@@ -5679,7 +5761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -5687,12 +5769,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
@@ -5705,13 +5787,13 @@
       <c r="E13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
         <v>211</v>
       </c>
@@ -5724,11 +5806,11 @@
       <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
         <v>57</v>
       </c>
@@ -5739,11 +5821,11 @@
         <v>33</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
@@ -5756,13 +5838,13 @@
       <c r="E16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -5775,13 +5857,13 @@
       <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
@@ -5792,11 +5874,11 @@
         <v>33</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
@@ -5809,16 +5891,16 @@
       <c r="E19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
@@ -5826,7 +5908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
@@ -5834,12 +5916,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
         <v>30</v>
       </c>
@@ -5849,15 +5931,15 @@
       <c r="D26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="2:9">
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
         <v>130</v>
       </c>
@@ -5867,13 +5949,13 @@
       <c r="D27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="2:9">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B28" s="1" t="s">
         <v>119</v>
       </c>
@@ -5883,20 +5965,20 @@
       <c r="D28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="30" spans="2:9">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B30" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>128</v>
       </c>
@@ -5927,33 +6009,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K37"/>
+  <dimension ref="B2:K40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
@@ -5961,7 +6043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -5969,12 +6051,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
@@ -5984,15 +6066,15 @@
       <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
         <v>165</v>
       </c>
@@ -6002,13 +6084,13 @@
       <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
         <v>166</v>
       </c>
@@ -6018,13 +6100,13 @@
       <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
         <v>167</v>
       </c>
@@ -6034,15 +6116,15 @@
       <c r="D13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
         <v>168</v>
       </c>
@@ -6052,13 +6134,13 @@
       <c r="D14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
         <v>169</v>
       </c>
@@ -6068,13 +6150,13 @@
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>170</v>
       </c>
@@ -6084,321 +6166,372 @@
       <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B18" s="9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B19" s="12" t="s">
         <v>171</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21" t="s">
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B20" s="14" t="s">
         <v>214</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="23">
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="24">
         <v>400</v>
       </c>
-      <c r="K20" s="23"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B21" s="14" t="s">
         <v>182</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="23">
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="24">
         <v>400</v>
       </c>
-      <c r="K21" s="23"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B22" s="14" t="s">
         <v>183</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="23">
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="24">
         <v>415</v>
       </c>
-      <c r="K22" s="23"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B23" s="14" t="s">
         <v>210</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="23">
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="24">
         <v>500</v>
       </c>
-      <c r="K23" s="23"/>
-    </row>
-    <row r="25" spans="2:11">
+      <c r="K23" s="24"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" s="9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B26" s="12" t="s">
         <v>174</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" s="11" t="s">
         <v>187</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-    </row>
-    <row r="28" spans="2:11" ht="27">
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+    </row>
+    <row r="28" spans="2:11" ht="36" x14ac:dyDescent="0.45">
       <c r="B28" s="19" t="s">
         <v>222</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-    </row>
-    <row r="29" spans="2:11" ht="27">
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+    </row>
+    <row r="29" spans="2:11" ht="36" x14ac:dyDescent="0.45">
       <c r="B29" s="11" t="s">
         <v>224</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-    </row>
-    <row r="30" spans="2:11">
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30" s="15" t="s">
         <v>201</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" s="15" t="s">
         <v>225</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-    </row>
-    <row r="32" spans="2:11">
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" s="15" t="s">
         <v>202</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-    </row>
-    <row r="33" spans="2:9" ht="27">
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+    </row>
+    <row r="33" spans="2:9" ht="36" x14ac:dyDescent="0.45">
       <c r="B33" s="15" t="s">
         <v>226</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" spans="2:9">
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B34" s="7" t="s">
         <v>186</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-    </row>
-    <row r="35" spans="2:9">
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B35" s="15" t="s">
         <v>203</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="16" t="s">
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+    </row>
+    <row r="36" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="27"/>
+    </row>
+    <row r="37" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B40" s="16" t="s">
         <v>212</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="30">
+    <mergeCell ref="D38:I38"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="D37:I37"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D22:I22"/>
     <mergeCell ref="D31:I31"/>
     <mergeCell ref="D33:I33"/>
     <mergeCell ref="D34:I34"/>
     <mergeCell ref="D35:I35"/>
     <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D23:I23"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="D27:I27"/>
     <mergeCell ref="D28:I28"/>
-    <mergeCell ref="D22:I22"/>
     <mergeCell ref="D30:I30"/>
     <mergeCell ref="D32:I32"/>
     <mergeCell ref="D29:I29"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>